<commit_message>
chenged name of rack in prac2.xl
</commit_message>
<xml_diff>
--- a/practice2.xlsx
+++ b/practice2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ar vr\user_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E215D-ABE0-443C-A331-83A5537E27DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F9E0CA-3CA8-499B-B9A8-92100A696F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>51 AA 1,2,3</t>
   </si>
@@ -364,9 +364,6 @@
     <t>31 AN 1,2,3,4,5</t>
   </si>
   <si>
-    <t>41 AL 1,2,3,4,5</t>
-  </si>
-  <si>
     <t>42 AQ 1,2,3,4,5</t>
   </si>
   <si>
@@ -380,6 +377,18 @@
   </si>
   <si>
     <t>100 AB 1,2,3</t>
+  </si>
+  <si>
+    <t>75 AP 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>76 AL 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>77 AL 1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>79 AP 1,2,3,4,5</t>
   </si>
 </sst>
 </file>
@@ -841,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1046,7 @@
         <v>24</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W11" s="2"/>
     </row>
@@ -1573,7 +1582,7 @@
         <v>109</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>110</v>
@@ -1583,7 +1592,7 @@
         <v>111</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>112</v>
@@ -1593,10 +1602,10 @@
         <v>113</v>
       </c>
       <c r="M23" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="N23" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="N23" s="10" t="s">
-        <v>115</v>
       </c>
       <c r="O23" s="10"/>
       <c r="P23" s="11" t="s">
@@ -1604,17 +1613,17 @@
       </c>
       <c r="Q23" s="12"/>
       <c r="R23" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S23" s="10"/>
       <c r="T23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="U23" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="U23" s="10" t="s">
-        <v>118</v>
-      </c>
       <c r="V23" s="11" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="W23" s="2"/>
     </row>

</xml_diff>